<commit_message>
Aded presentation, final dissertation copy, and a restructuring of some folders and rewriting of some readmes
</commit_message>
<xml_diff>
--- a/data/processed/study/quantitative.xlsx
+++ b/data/processed/study/quantitative.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Turne\Documents\Project Folder\Project Repo\data\processed\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6F3635-8EC4-4986-B338-738250A51071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4CCE15-2942-464B-A8DB-FB55B7FF2E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7692" yWindow="972" windowWidth="22200" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1512" yWindow="3672" windowWidth="22200" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Number of successful auths</t>
   </si>
   <si>
-    <t>Number of attempts</t>
-  </si>
-  <si>
-    <t>Success rate</t>
-  </si>
-  <si>
     <t>Participant ID</t>
   </si>
   <si>
@@ -62,6 +56,27 @@
   </si>
   <si>
     <t>Pendant</t>
+  </si>
+  <si>
+    <t>Mean Time (sec)</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Max Time</t>
+  </si>
+  <si>
+    <t>Min Time</t>
+  </si>
+  <si>
+    <t>Success rate (across authentication)</t>
+  </si>
+  <si>
+    <t>Success rate (across attempt)</t>
+  </si>
+  <si>
+    <t>Number of attempted auths</t>
   </si>
 </sst>
 </file>
@@ -379,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,33 +405,50 @@
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="24.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -428,13 +460,28 @@
         <f>C2/D2*100</f>
         <v>38.70967741935484</v>
       </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="H2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="I2">
+        <v>8.09</v>
+      </c>
+      <c r="J2">
+        <v>3.67</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>44</v>
@@ -446,13 +493,28 @@
         <f t="shared" ref="E3:E4" si="0">C3/D3*100</f>
         <v>88</v>
       </c>
+      <c r="F3">
+        <v>53.66</v>
+      </c>
+      <c r="G3">
+        <v>15.51</v>
+      </c>
+      <c r="H3">
+        <v>2.65</v>
+      </c>
+      <c r="I3">
+        <v>5.16</v>
+      </c>
+      <c r="J3">
+        <v>2.68</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>11</v>
@@ -464,12 +526,27 @@
         <f t="shared" si="0"/>
         <v>61.111111111111114</v>
       </c>
+      <c r="F4">
+        <v>23.4</v>
+      </c>
+      <c r="G4">
+        <v>12.29</v>
+      </c>
+      <c r="H4">
+        <v>2.29</v>
+      </c>
+      <c r="I4">
+        <v>5.47</v>
+      </c>
+      <c r="J4">
+        <v>3.49</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <f>AVERAGE(E2:E4)</f>
         <v>62.606929510155318</v>
       </c>

</xml_diff>